<commit_message>
Update School Reportcard - Inexperienced Teachers.xlsx
</commit_message>
<xml_diff>
--- a/data/FLDOE/School Reportcard - Inexperienced Teachers.xlsx
+++ b/data/FLDOE/School Reportcard - Inexperienced Teachers.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/41d025303327e0f0/Documents/GitHub/hillsborough_grades/data/FLDOE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBCFA536-4DB9-4A7A-A33B-A501729BEDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{DBCFA536-4DB9-4A7A-A33B-A501729BEDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C939D8C-A751-477E-BB39-E1DFCE1E5A6A}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{F5DF7167-33E2-4B7E-9F6C-30FFD989D8AF}"/>
   </bookViews>
   <sheets>
     <sheet name="DF Schools" sheetId="1" r:id="rId1"/>
     <sheet name="Hillsborough" sheetId="2" r:id="rId2"/>
+    <sheet name="Source" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="80">
   <si>
     <t>School Name</t>
   </si>
@@ -268,6 +269,15 @@
   </si>
   <si>
     <t>Non-Title I and Low Minority Schools</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>https://edudata.fldoe.org/</t>
   </si>
 </sst>
 </file>
@@ -623,11 +633,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA554FD-6E1F-49CC-8E9D-B65A41FAA933}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -653,6 +666,9 @@
       <c r="C2">
         <v>0.33300000000000002</v>
       </c>
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -664,6 +680,9 @@
       <c r="C3">
         <v>0.48</v>
       </c>
+      <c r="D3" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -672,6 +691,12 @@
       <c r="B4">
         <v>128</v>
       </c>
+      <c r="C4">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="D4" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -680,6 +705,12 @@
       <c r="B5">
         <v>282</v>
       </c>
+      <c r="C5">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="D5" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -688,6 +719,12 @@
       <c r="B6">
         <v>441</v>
       </c>
+      <c r="C6">
+        <v>0.115</v>
+      </c>
+      <c r="D6" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -696,6 +733,12 @@
       <c r="B7">
         <v>641</v>
       </c>
+      <c r="C7">
+        <v>0.219</v>
+      </c>
+      <c r="D7" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -704,6 +747,12 @@
       <c r="B8">
         <v>962</v>
       </c>
+      <c r="C8">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="D8" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -712,6 +761,12 @@
       <c r="B9">
         <v>1361</v>
       </c>
+      <c r="C9">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="D9" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -720,6 +775,9 @@
       <c r="B10">
         <v>1481</v>
       </c>
+      <c r="C10">
+        <v>0.379</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -728,6 +786,12 @@
       <c r="B11">
         <v>1761</v>
       </c>
+      <c r="C11">
+        <v>0.19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -736,6 +800,9 @@
       <c r="B12">
         <v>1951</v>
       </c>
+      <c r="C12">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -744,6 +811,12 @@
       <c r="B13">
         <v>2041</v>
       </c>
+      <c r="C13">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="D13" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -752,6 +825,12 @@
       <c r="B14">
         <v>2201</v>
       </c>
+      <c r="C14">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="D14" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -759,6 +838,12 @@
       </c>
       <c r="B15">
         <v>2261</v>
+      </c>
+      <c r="C15">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="D15" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1506,4 +1591,22 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E063E3-D156-415D-A47E-D554352EC55C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>